<commit_message>
add new ecoli studies and NB ratio analysis
</commit_message>
<xml_diff>
--- a/results/escherichia_coli/ICA_Study/reaction_sensitivity_EX_acgam_e13.33-EX_phe__L_e15.0.xlsx
+++ b/results/escherichia_coli/ICA_Study/reaction_sensitivity_EX_acgam_e13.33-EX_phe__L_e15.0.xlsx
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>604</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>608</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4">
@@ -476,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>599</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5">
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>594</v>
+        <v>515</v>
       </c>
     </row>
     <row r="6">
@@ -498,7 +498,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>588</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7">
@@ -509,7 +509,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>577</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8">
@@ -520,7 +520,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>575</v>
+        <v>500</v>
       </c>
     </row>
     <row r="9">
@@ -531,7 +531,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>561</v>
+        <v>485</v>
       </c>
     </row>
     <row r="10">
@@ -542,7 +542,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>552</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11">
@@ -553,7 +553,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>546</v>
+        <v>483</v>
       </c>
     </row>
     <row r="12">
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>537</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13">
@@ -575,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>534</v>
+        <v>456</v>
       </c>
     </row>
     <row r="14">
@@ -586,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>531</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15">
@@ -597,7 +597,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>529</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16">
@@ -608,7 +608,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>524</v>
+        <v>450</v>
       </c>
     </row>
     <row r="17">
@@ -619,7 +619,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>516</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18">
@@ -630,7 +630,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>513</v>
+        <v>439</v>
       </c>
     </row>
     <row r="19">
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>510</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20">
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>507</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>574</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3">
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>565</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4">
@@ -716,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>556</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5">
@@ -727,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>555</v>
+        <v>639</v>
       </c>
     </row>
     <row r="6">
@@ -738,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>550</v>
+        <v>642</v>
       </c>
     </row>
     <row r="7">
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>546</v>
+        <v>631</v>
       </c>
     </row>
     <row r="8">
@@ -760,7 +760,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>540</v>
+        <v>628</v>
       </c>
     </row>
     <row r="9">
@@ -771,7 +771,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>546</v>
+        <v>630</v>
       </c>
     </row>
     <row r="10">
@@ -782,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>536</v>
+        <v>631</v>
       </c>
     </row>
     <row r="11">
@@ -793,7 +793,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>541</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12">
@@ -804,7 +804,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>543</v>
+        <v>628</v>
       </c>
     </row>
     <row r="13">
@@ -815,7 +815,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>539</v>
+        <v>635</v>
       </c>
     </row>
     <row r="14">
@@ -826,7 +826,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>538</v>
+        <v>632</v>
       </c>
     </row>
     <row r="15">
@@ -837,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>535</v>
+        <v>627</v>
       </c>
     </row>
     <row r="16">
@@ -848,7 +848,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>534</v>
+        <v>630</v>
       </c>
     </row>
     <row r="17">
@@ -859,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>534</v>
+        <v>629</v>
       </c>
     </row>
     <row r="18">
@@ -870,7 +870,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>542</v>
+        <v>632</v>
       </c>
     </row>
     <row r="19">
@@ -881,7 +881,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>538</v>
+        <v>634</v>
       </c>
     </row>
     <row r="20">
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>542</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>